<commit_message>
more errors, updated EBNF, completed Gantt Chart
</commit_message>
<xml_diff>
--- a/Gantt Chart.xlsx
+++ b/Gantt Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesthompson 1/GF2-Team-11/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4EDA1B-17CA-EB4D-8F95-E2E595E91B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DB6AD0-305B-3B43-9BBF-6728C6687398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{C3028E7F-4077-5341-994D-941B531B2831}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{C3028E7F-4077-5341-994D-941B531B2831}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Write Scanner Module</t>
   </si>
@@ -48,18 +48,6 @@
     <t>Write GUI Module</t>
   </si>
   <si>
-    <t>Test Scanner</t>
-  </si>
-  <si>
-    <t>Test Parse</t>
-  </si>
-  <si>
-    <t>Test Names</t>
-  </si>
-  <si>
-    <t>Test GUI</t>
-  </si>
-  <si>
     <t>Maintenance</t>
   </si>
   <si>
@@ -67,6 +55,45 @@
   </si>
   <si>
     <t>Final Report Deadline</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>Neelay</t>
+  </si>
+  <si>
+    <t>Write Names Unit Tests</t>
+  </si>
+  <si>
+    <t>Write Scannner Unit Tests</t>
+  </si>
+  <si>
+    <t>Debug Names</t>
+  </si>
+  <si>
+    <t>Debug Scanner</t>
+  </si>
+  <si>
+    <t>Write Parse Unit Tests</t>
+  </si>
+  <si>
+    <t>Write GUI Unit Tests</t>
+  </si>
+  <si>
+    <t>Debug Parse</t>
+  </si>
+  <si>
+    <t>Debug GUI</t>
+  </si>
+  <si>
+    <t>Integrate Modules</t>
+  </si>
+  <si>
+    <t>All</t>
   </si>
 </sst>
 </file>
@@ -90,12 +117,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD4B7FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -110,18 +161,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFD4B7FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -430,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3CC6132-9492-E649-A89F-B6AC63929F5C}">
-  <dimension ref="B2:T14"/>
+  <dimension ref="B2:T23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -445,10 +506,10 @@
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.2">
       <c r="N2" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.2">
@@ -509,63 +570,145 @@
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
       <c r="N4" s="3"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
       <c r="N5" s="3"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>2</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
       <c r="N6" s="3"/>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>3</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
       <c r="N7" s="3"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>4</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F8" s="7"/>
       <c r="N8" s="3"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>5</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="F9" s="5"/>
       <c r="N9" s="3"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>6</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
       <c r="N10" s="3"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>7</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
       <c r="N11" s="3"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="N12" s="3"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="N13" s="3"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="N14" s="3"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="C19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="N12" s="3"/>
-    </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="N13" s="3"/>
-    </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="N14" s="3"/>
+      <c r="E19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="D23" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>